<commit_message>
V1.1 Adding two additional test cases and some updates according two the review
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_ADMINCONSTRAINS.xlsx
+++ b/LH_TESTCASES/LH_TC_ADMINCONSTRAINS.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Preconditions</t>
   </si>
@@ -210,9 +210,6 @@
     <t>TC_ADM_005</t>
   </si>
   <si>
-    <t>SRS-ADM-003</t>
-  </si>
-  <si>
     <t>Verify admin can delete a user by username.</t>
   </si>
   <si>
@@ -228,18 +225,65 @@
     <t xml:space="preserve">Admin is logged in, a user exists </t>
   </si>
   <si>
+    <t>TC_ADM_006</t>
+  </si>
+  <si>
     <t>1_Log in as admin.
-2_Navigate to user 3_management section.
-4_Search for user by username.
+2_Navigate to user management section.
+4_Search for user by  valid username.
 5_Click “Delete” button.
 6_Confirm deletion</t>
   </si>
   <si>
+    <t>user name (eg.eman21)</t>
+  </si>
+  <si>
+    <t>User id (ex:U001)</t>
+  </si>
+  <si>
     <t>1_Log in as admin.
-2_Navigate to user 3_management section.
-4_Search for user by .
+2_Navigate to user management section.
+4_Search for user by valid ID.
 5_Click “Delete” button.
 6_Confirm deletion</t>
+  </si>
+  <si>
+    <t>Verify admin can not delete 
+       non-existent user (non exist user name)</t>
+  </si>
+  <si>
+    <t>TC_ADM_007</t>
+  </si>
+  <si>
+    <t>Admin is logged in, a user name is notexist</t>
+  </si>
+  <si>
+    <t>Admin is logged in, a user idis notexist</t>
+  </si>
+  <si>
+    <t>1_Log in as admin.
+2_Navigate to user management section.
+4_Search for user by non existant user name .
+5_Click “Delete” button.
+6_Confirm deletion</t>
+  </si>
+  <si>
+    <t>Error message("No users with this information")</t>
+  </si>
+  <si>
+    <t>1_Log in as admin.
+2_Navigate to user management section.
+4_Search for user by non existant user id.
+5_Click “Delete” button.
+6_Confirm deletion</t>
+  </si>
+  <si>
+    <t>V1.1</t>
+  </si>
+  <si>
+    <t>_Edit the id for LH_SRS_ADM_003 to
+LH_SRS_ADM_002
+_add more two test cases for LH_SRS_ADM_002</t>
   </si>
 </sst>
 </file>
@@ -416,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -451,6 +495,39 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -468,36 +545,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,19 +870,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="31" style="5" customWidth="1"/>
     <col min="2" max="2" width="28" style="1" customWidth="1"/>
-    <col min="3" max="3" width="70.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45" style="1" customWidth="1"/>
+    <col min="3" max="3" width="78.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="61.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="31.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="29" customWidth="1"/>
-    <col min="7" max="7" width="54.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="23" customWidth="1"/>
+    <col min="7" max="7" width="62.42578125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.7109375" style="17"/>
     <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
@@ -847,42 +894,42 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
-      <c r="F1" s="28"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="23"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -936,19 +983,19 @@
       <c r="C9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G9" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I9" s="27"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="1:10" ht="147" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
@@ -960,13 +1007,13 @@
       <c r="C10" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G10" s="15" t="s">
@@ -983,94 +1030,132 @@
       <c r="C11" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="25" t="s">
+      <c r="F11" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G11" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="31" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+    <row r="12" spans="1:10" s="25" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="C12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="33"/>
+      <c r="F12" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:10" s="15" customFormat="1" ht="168" x14ac:dyDescent="0.25">
-      <c r="A13" s="30" t="s">
-        <v>43</v>
+      <c r="A13" s="24" t="s">
+        <v>29</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="15" t="s">
+      <c r="I13" s="21"/>
+    </row>
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="209.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="27"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F14" s="25" t="s">
+      <c r="G14" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="21"/>
+    </row>
+    <row r="15" spans="1:10" ht="168" x14ac:dyDescent="0.35">
+      <c r="A15" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="19" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F15" s="25" t="s">
+      <c r="G15" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="F16" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F16" s="25" t="s">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F17" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F17" s="25" t="s">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F18" s="25" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.35">
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="19" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1105,7 +1190,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1142,14 +1227,23 @@
       </c>
       <c r="D2" s="13">
         <f ca="1">TODAY()</f>
-        <v>45766</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="13">
+        <f ca="1">TODAY()</f>
+        <v>45769</v>
+      </c>
     </row>
     <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>

</xml_diff>

<commit_message>
V1.1 reuploading after review
there was  a small syntax mistake; instead of user id, it was written user name
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_ADMINCONSTRAINS.xlsx
+++ b/LH_TESTCASES/LH_TC_ADMINCONSTRAINS.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Preconditions</t>
   </si>
@@ -258,9 +258,6 @@
     <t>Admin is logged in, a user name is notexist</t>
   </si>
   <si>
-    <t>Admin is logged in, a user idis notexist</t>
-  </si>
-  <si>
     <t>1_Log in as admin.
 2_Navigate to user management section.
 4_Search for user by non existant user name .
@@ -284,6 +281,13 @@
     <t>_Edit the id for LH_SRS_ADM_003 to
 LH_SRS_ADM_002
 _add more two test cases for LH_SRS_ADM_002</t>
+  </si>
+  <si>
+    <t>Verify admin can not delete 
+       non-existent user (non exist user id)</t>
+  </si>
+  <si>
+    <t>Admin is logged in, a user id is notexist</t>
   </si>
 </sst>
 </file>
@@ -870,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -997,7 +1001,7 @@
       </c>
       <c r="I9" s="21"/>
     </row>
-    <row r="10" spans="1:10" ht="147" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="126" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>22</v>
       </c>
@@ -1020,7 +1024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="147" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" ht="126" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
@@ -1067,7 +1071,7 @@
       </c>
       <c r="I12" s="27"/>
     </row>
-    <row r="13" spans="1:10" s="15" customFormat="1" ht="168" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="15" customFormat="1" ht="147" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>29</v>
       </c>
@@ -1105,13 +1109,13 @@
         <v>55</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F14" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I14" s="21"/>
     </row>
@@ -1123,19 +1127,19 @@
         <v>54</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F15" s="19" t="s">
         <v>40</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -1232,13 +1236,13 @@
     </row>
     <row r="3" spans="1:4" s="9" customFormat="1" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" s="13">
         <f ca="1">TODAY()</f>

</xml_diff>